<commit_message>
Review all CDDs and update GDD review sheet Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/GDD/Review.xlsx
+++ b/Software Specification/Architecture/GDD/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Review point</t>
   </si>
@@ -72,6 +72,15 @@
     <t>Switch_errorRead:
 This function will be called by whom ?
 If it will be called by the application so application shall not know any thing about the PORT number or assigned pin number, application shall request to read switch number 1 or 2 or 3 .. etc</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Mali 13/3/2020: Point still open</t>
   </si>
 </sst>
 </file>
@@ -155,7 +164,136 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -542,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -586,9 +724,11 @@
       <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
@@ -605,6 +745,9 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F3" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5">
@@ -616,9 +759,11 @@
       <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
@@ -631,9 +776,11 @@
       <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
@@ -646,9 +793,11 @@
       <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30">
@@ -691,9 +840,11 @@
       <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="75">
@@ -706,28 +857,30 @@
       <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="containsText" dxfId="9" priority="98" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="24" priority="98" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="99" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="23" priority="99" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="100" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="22" priority="100" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="cellIs" dxfId="6" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="93" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="94" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>